<commit_message>
Pushing final versions of .ipynb files
</commit_message>
<xml_diff>
--- a/output_romney.xlsx
+++ b/output_romney.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d67fcbc81130eed1/UIC/Fall_2023/CS_583/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_08B5A9E49D4040FE671BC45752245E3FB48F8CAD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8CD7882-727D-4FB4-9F89-6D45F8B7A14F}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_E8A924241E706AFF671BC45752245E3FE402DA1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3544B6AE-1931-4B4D-9F42-DC84E010C3AD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Romney" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -406,7 +406,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="130.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>